<commit_message>
Updating exec time table
</commit_message>
<xml_diff>
--- a/tests/polybench-c-3.2/results/exec-time-table-full-polybench.xlsx
+++ b/tests/polybench-c-3.2/results/exec-time-table-full-polybench.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="8820" yWindow="420" windowWidth="16180" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>correlation</t>
   </si>
@@ -114,17 +114,44 @@
     <t>Benchmark</t>
   </si>
   <si>
-    <t>opt/clean</t>
+    <t>ignore-alias /clean</t>
+  </si>
+  <si>
+    <t>opt /clean</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -234,18 +261,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,8 +315,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -591,271 +663,366 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" ht="30" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>31</v>
       </c>
+      <c r="C1" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="10">
+        <v>0.99684918725841232</v>
+      </c>
+      <c r="C2" s="4">
         <v>1.006434278</v>
       </c>
-      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="6">
+        <v>0.99786251461118336</v>
+      </c>
+      <c r="C3" s="6">
         <v>1.006616041</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
+        <v>0.99885250667016012</v>
+      </c>
+      <c r="C4" s="6">
         <v>0.99984814399999999</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="6">
+        <v>1.0115700171216659</v>
+      </c>
+      <c r="C5" s="6">
         <v>1.019268796</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
+        <v>2.0359277488759853</v>
+      </c>
+      <c r="C6" s="6">
         <v>2.0986942119999998</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
+        <v>0.93816242191146082</v>
+      </c>
+      <c r="C7" s="6">
         <v>0.93550735299999999</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
+        <v>0.99078206538850777</v>
+      </c>
+      <c r="C8" s="6">
         <v>1.019051223</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
+        <v>0.90427142189875376</v>
+      </c>
+      <c r="C9" s="6">
         <v>0.92485392700000002</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
+        <v>0.97385654844127834</v>
+      </c>
+      <c r="C10" s="6">
         <v>0.99569216900000002</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
+        <v>0.43822490563299604</v>
+      </c>
+      <c r="C11" s="6">
         <v>0.426479952</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
+        <v>1.1361512416553816</v>
+      </c>
+      <c r="C12" s="6">
         <v>1.153806119</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
+        <v>0.28315643691924919</v>
+      </c>
+      <c r="C13" s="6">
         <v>0.27416405100000002</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
+        <v>0.99421835594677654</v>
+      </c>
+      <c r="C14" s="6">
         <v>0.97799745299999996</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
+        <v>0.97185107990721742</v>
+      </c>
+      <c r="C15" s="6">
         <v>0.96705886699999999</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
+        <v>0.94683263407344598</v>
+      </c>
+      <c r="C16" s="6">
         <v>0.94682389199999994</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
+        <v>0.9856877599300119</v>
+      </c>
+      <c r="C17" s="6">
         <v>1.0030598470000001</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
+        <v>1.0015622033817697</v>
+      </c>
+      <c r="C18" s="6">
         <v>0.98033155599999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
+        <v>1.0061330375189017</v>
+      </c>
+      <c r="C19" s="6">
         <v>1.0396443950000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="7" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
+        <v>0.97086344982154482</v>
+      </c>
+      <c r="C20" s="6">
         <v>1.078307226</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
+        <v>1.0041683420844889</v>
+      </c>
+      <c r="C21" s="6">
         <v>0.98877519599999997</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
+        <v>0.99792136700503431</v>
+      </c>
+      <c r="C22" s="6">
         <v>0.95103869699999999</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="6">
+        <v>1.0025008857060866</v>
+      </c>
+      <c r="C23" s="6">
         <v>1.008412021</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="7" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="6">
+        <v>1.0011620401056651</v>
+      </c>
+      <c r="C24" s="6">
         <v>0.99759054700000005</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="6">
+        <v>2.1359834390407868</v>
+      </c>
+      <c r="C25" s="6">
         <v>2.59568434</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26" s="6">
+        <v>1.0012426025070573</v>
+      </c>
+      <c r="C26" s="6">
         <v>0.66453413900000002</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="6">
+        <v>1.0011265099134947</v>
+      </c>
+      <c r="C27" s="6">
         <v>0.98927283499999996</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="6">
+        <v>1.0028817636109317</v>
+      </c>
+      <c r="C28" s="6">
         <v>1.0066804760000001</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="6">
+        <v>1.7536201903267143</v>
+      </c>
+      <c r="C29" s="6">
         <v>2.3063784360000001</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="6">
+        <v>1.7732759876044697</v>
+      </c>
+      <c r="C30" s="6">
         <v>1.7707284409999999</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="8">
+        <v>0.99549626378357969</v>
+      </c>
+      <c r="C31" s="8">
         <v>1.0261859470000001</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>